<commit_message>
0.1.3: Enable search listTmpdir to import list classes.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectTsResourceBundle.xlsx
+++ b/meta/program/BlancoValueObjectTsResourceBundle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C56D1D9-D76E-0345-934A-F933B8C725F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90ED29C-C26A-DD4A-B607-F6820BFA9FA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="113">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -621,6 +621,26 @@
   </si>
   <si>
     <t>META2XML.ELEMENT_COMMON_TS</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.ERR007</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>クラス名検索用オブジェクトを保管するための引数にnullが与えられました。</t>
+    <rPh sb="4" eb="7">
+      <t xml:space="preserve">ケンサクヨウ </t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">ホカンスル </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">ヒキスウニ </t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t xml:space="preserve">アタエラレマシタ。 </t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1047,6 +1067,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1062,12 +1088,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1479,10 +1499,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1599,25 +1619,25 @@
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="37"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="39"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
       <c r="G14" s="18"/>
@@ -2211,8 +2231,12 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B55" s="23"/>
-      <c r="C55" s="20"/>
+      <c r="B55" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>112</v>
+      </c>
       <c r="D55" s="21"/>
       <c r="E55" s="21"/>
       <c r="F55" s="21"/>
@@ -2223,12 +2247,8 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B56" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="B56" s="23"/>
+      <c r="C56" s="20"/>
       <c r="D56" s="21"/>
       <c r="E56" s="21"/>
       <c r="F56" s="21"/>
@@ -2240,10 +2260,10 @@
         <v>43</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="21"/>
@@ -2256,10 +2276,10 @@
         <v>44</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="21"/>
@@ -2271,8 +2291,12 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="20"/>
+      <c r="B59" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>58</v>
+      </c>
       <c r="D59" s="21"/>
       <c r="E59" s="21"/>
       <c r="F59" s="21"/>
@@ -2283,12 +2307,8 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B60" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="20" t="s">
-        <v>78</v>
-      </c>
+      <c r="B60" s="23"/>
+      <c r="C60" s="20"/>
       <c r="D60" s="21"/>
       <c r="E60" s="21"/>
       <c r="F60" s="21"/>
@@ -2300,10 +2320,10 @@
         <v>47</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
@@ -2316,10 +2336,10 @@
         <v>48</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="D62" s="21"/>
       <c r="E62" s="21"/>
@@ -2331,8 +2351,12 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="20"/>
+      <c r="B63" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>79</v>
+      </c>
       <c r="D63" s="21"/>
       <c r="E63" s="21"/>
       <c r="F63" s="21"/>
@@ -2343,12 +2367,8 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B64" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C64" s="20" t="s">
-        <v>80</v>
-      </c>
+      <c r="B64" s="23"/>
+      <c r="C64" s="20"/>
       <c r="D64" s="21"/>
       <c r="E64" s="21"/>
       <c r="F64" s="21"/>
@@ -2360,10 +2380,10 @@
         <v>51</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D65" s="21"/>
       <c r="E65" s="21"/>
@@ -2376,10 +2396,10 @@
         <v>52</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="21"/>
@@ -2392,10 +2412,10 @@
         <v>53</v>
       </c>
       <c r="B67" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D67" s="21"/>
       <c r="E67" s="21"/>
@@ -2407,8 +2427,12 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B68" s="23"/>
-      <c r="C68" s="20"/>
+      <c r="B68" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>83</v>
+      </c>
       <c r="D68" s="21"/>
       <c r="E68" s="21"/>
       <c r="F68" s="21"/>
@@ -2419,12 +2443,8 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B69" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C69" s="20" t="s">
-        <v>84</v>
-      </c>
+      <c r="B69" s="23"/>
+      <c r="C69" s="20"/>
       <c r="D69" s="21"/>
       <c r="E69" s="21"/>
       <c r="F69" s="21"/>
@@ -2436,10 +2456,10 @@
         <v>56</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D70" s="21"/>
       <c r="E70" s="21"/>
@@ -2452,10 +2472,10 @@
         <v>57</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D71" s="21"/>
       <c r="E71" s="21"/>
@@ -2468,10 +2488,10 @@
         <v>58</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D72" s="21"/>
       <c r="E72" s="21"/>
@@ -2483,8 +2503,12 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B73" s="23"/>
-      <c r="C73" s="20"/>
+      <c r="B73" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C73" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="D73" s="21"/>
       <c r="E73" s="21"/>
       <c r="F73" s="21"/>
@@ -2495,12 +2519,8 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B74" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C74" s="20" t="s">
-        <v>87</v>
-      </c>
+      <c r="B74" s="23"/>
+      <c r="C74" s="20"/>
       <c r="D74" s="21"/>
       <c r="E74" s="21"/>
       <c r="F74" s="21"/>
@@ -2511,8 +2531,12 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B75" s="23"/>
-      <c r="C75" s="20"/>
+      <c r="B75" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C75" s="20" t="s">
+        <v>87</v>
+      </c>
       <c r="D75" s="21"/>
       <c r="E75" s="21"/>
       <c r="F75" s="21"/>
@@ -2524,9 +2548,7 @@
         <v>62</v>
       </c>
       <c r="B76" s="23"/>
-      <c r="C76" s="20" t="s">
-        <v>72</v>
-      </c>
+      <c r="C76" s="20"/>
       <c r="D76" s="21"/>
       <c r="E76" s="21"/>
       <c r="F76" s="21"/>
@@ -2539,7 +2561,7 @@
       </c>
       <c r="B77" s="23"/>
       <c r="C77" s="20" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="21"/>
@@ -2553,7 +2575,7 @@
       </c>
       <c r="B78" s="23"/>
       <c r="C78" s="20" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="21"/>
@@ -2566,7 +2588,9 @@
         <v>65</v>
       </c>
       <c r="B79" s="23"/>
-      <c r="C79" s="20"/>
+      <c r="C79" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="D79" s="21"/>
       <c r="E79" s="21"/>
       <c r="F79" s="21"/>
@@ -2577,12 +2601,8 @@
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B80" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="C80" s="20" t="s">
-        <v>89</v>
-      </c>
+      <c r="B80" s="23"/>
+      <c r="C80" s="20"/>
       <c r="D80" s="21"/>
       <c r="E80" s="21"/>
       <c r="F80" s="21"/>
@@ -2590,14 +2610,14 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="28">
-        <f t="shared" ref="A81:A87" si="1">A80+1</f>
+        <f t="shared" ref="A81:A88" si="1">A80+1</f>
         <v>67</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="21"/>
@@ -2610,10 +2630,10 @@
         <v>68</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="21"/>
@@ -2626,10 +2646,10 @@
         <v>69</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="21"/>
@@ -2642,10 +2662,10 @@
         <v>70</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="21"/>
@@ -2658,10 +2678,10 @@
         <v>71</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21"/>
@@ -2674,10 +2694,10 @@
         <v>72</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="21"/>
@@ -2690,24 +2710,40 @@
         <v>73</v>
       </c>
       <c r="B87" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C87" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D87" s="21"/>
+      <c r="E87" s="21"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="22"/>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="28">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B88" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C87" s="20" t="s">
+      <c r="C88" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="D87" s="40"/>
-      <c r="E87" s="40"/>
-      <c r="F87" s="40"/>
-      <c r="G87" s="41"/>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="29"/>
-      <c r="B88" s="24"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="26"/>
-      <c r="E88" s="26"/>
-      <c r="F88" s="26"/>
-      <c r="G88" s="27"/>
+      <c r="D88" s="34"/>
+      <c r="E88" s="34"/>
+      <c r="F88" s="34"/>
+      <c r="G88" s="35"/>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="29"/>
+      <c r="B89" s="24"/>
+      <c r="C89" s="25"/>
+      <c r="D89" s="26"/>
+      <c r="E89" s="26"/>
+      <c r="F89" s="26"/>
+      <c r="G89" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>